<commit_message>
Semana 10 de 2024
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -441,6 +441,22 @@
         <v>395</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
seman 13 2024 boletin
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -462,7 +462,15 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>635</v>
+        <v>680</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>478</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
semana 14 de 2024
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -470,7 +470,15 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>478</v>
+        <v>490</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>734</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
semana 30 de 2024
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -513,6 +513,102 @@
         <v>419</v>
       </c>
     </row>
+    <row r="20">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>400</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
semana 31 de 2024
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -609,6 +609,14 @@
         <v>400</v>
       </c>
     </row>
+    <row r="32">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>474</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
semana 37 de 2024
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -617,6 +617,54 @@
         <v>474</v>
       </c>
     </row>
+    <row r="33">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>509</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
semana 38 de 2024
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -582,7 +582,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>348</v>
+        <v>381</v>
       </c>
     </row>
     <row r="29">
@@ -662,7 +662,15 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>509</v>
+        <v>537</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>612</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
semana 40 de 2024
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B39"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -673,6 +673,30 @@
         <v>612</v>
       </c>
     </row>
+    <row r="40">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
semana 42 de 2024
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -697,6 +697,14 @@
         <v>366</v>
       </c>
     </row>
+    <row r="43">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>502</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
semana 43 de 2024
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B43"/>
+  <dimension ref="A1:B45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -705,6 +705,22 @@
         <v>502</v>
       </c>
     </row>
+    <row r="44">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
semana 45 de 2024
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B45"/>
+  <dimension ref="A1:B46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -718,7 +718,15 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>63</v>
+        <v>444</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <v>580</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
smeana 46 de 2024
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B46"/>
+  <dimension ref="A1:B48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -726,7 +726,23 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>580</v>
+        <v>590</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
semana 48 de 2024
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B48"/>
+  <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -734,7 +734,7 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>462</v>
+        <v>478</v>
       </c>
     </row>
     <row r="48">
@@ -742,7 +742,23 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>8</v>
+        <v>474</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
semana 49 de 2024
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B50"/>
+  <dimension ref="A1:B51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -758,7 +758,15 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>3</v>
+        <v>425</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
semana 51 de 2024
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B51"/>
+  <dimension ref="A1:B53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -766,7 +766,23 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>84</v>
+        <v>564</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
semana 52 de 2024
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
@@ -374,7 +374,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>434</v>
+        <v>900</v>
       </c>
     </row>
     <row r="3">
@@ -382,7 +382,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>570</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="4">
@@ -390,7 +390,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>650</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="5">
@@ -398,7 +398,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>750</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="6">
@@ -406,7 +406,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>581</v>
+        <v>981</v>
       </c>
     </row>
     <row r="7">
@@ -414,7 +414,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>785</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="8">
@@ -422,7 +422,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>785</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="9">
@@ -430,7 +430,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>629</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="10">
@@ -438,7 +438,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>395</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="11">
@@ -446,7 +446,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>768</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="12">
@@ -454,7 +454,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>809</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="13">
@@ -462,7 +462,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>680</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="14">
@@ -470,7 +470,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>490</v>
+        <v>952</v>
       </c>
     </row>
     <row r="15">
@@ -478,7 +478,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>805</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="16">
@@ -486,7 +486,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>886</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="17">
@@ -494,7 +494,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>717</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="18">
@@ -502,7 +502,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>828</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="19">
@@ -510,7 +510,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>419</v>
+        <v>952</v>
       </c>
     </row>
     <row r="20">
@@ -518,7 +518,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>510</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="21">
@@ -526,7 +526,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>488</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="22">
@@ -534,7 +534,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>526</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="23">
@@ -542,7 +542,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>438</v>
+        <v>929</v>
       </c>
     </row>
     <row r="24">
@@ -550,7 +550,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>388</v>
+        <v>725</v>
       </c>
     </row>
     <row r="25">
@@ -558,7 +558,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>401</v>
+        <v>704</v>
       </c>
     </row>
     <row r="26">
@@ -566,7 +566,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>425</v>
+        <v>915</v>
       </c>
     </row>
     <row r="27">
@@ -574,7 +574,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>341</v>
+        <v>701</v>
       </c>
     </row>
     <row r="28">
@@ -582,7 +582,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>381</v>
+        <v>922</v>
       </c>
     </row>
     <row r="29">
@@ -590,7 +590,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>478</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="30">
@@ -598,7 +598,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>454</v>
+        <v>926</v>
       </c>
     </row>
     <row r="31">
@@ -606,7 +606,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>400</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="32">
@@ -614,7 +614,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>474</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="33">
@@ -622,7 +622,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>346</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="34">
@@ -630,7 +630,7 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>301</v>
+        <v>813</v>
       </c>
     </row>
     <row r="35">
@@ -638,7 +638,7 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>468</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="36">
@@ -646,7 +646,7 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>711</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="37">
@@ -654,7 +654,7 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>495</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="38">
@@ -662,7 +662,7 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>537</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="39">
@@ -670,7 +670,7 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>612</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="40">
@@ -678,7 +678,7 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <v>490</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="41">
@@ -686,7 +686,7 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>549</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="42">
@@ -694,7 +694,7 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>366</v>
+        <v>883</v>
       </c>
     </row>
     <row r="43">
@@ -702,7 +702,7 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>502</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="44">
@@ -710,7 +710,7 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>475</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="45">
@@ -718,7 +718,7 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>444</v>
+        <v>865</v>
       </c>
     </row>
     <row r="46">
@@ -726,7 +726,7 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>590</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="47">
@@ -734,7 +734,7 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>478</v>
+        <v>888</v>
       </c>
     </row>
     <row r="48">
@@ -742,7 +742,7 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>474</v>
+        <v>971</v>
       </c>
     </row>
     <row r="49">
@@ -750,7 +750,7 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>378</v>
+        <v>885</v>
       </c>
     </row>
     <row r="50">
@@ -758,7 +758,7 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>425</v>
+        <v>930</v>
       </c>
     </row>
     <row r="51">
@@ -766,7 +766,7 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>564</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="52">
@@ -774,7 +774,7 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <v>406</v>
+        <v>887</v>
       </c>
     </row>
     <row r="53">
@@ -782,7 +782,7 @@
         <v>52</v>
       </c>
       <c r="B53">
-        <v>36</v>
+        <v>903</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
semana 05 de 2025
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -398,7 +398,23 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>602</v>
+        <v>604</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
semana 06 de 2026
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -414,6 +414,14 @@
         <v>6</v>
       </c>
       <c r="B7">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
semana 11 de 2025
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -398,7 +398,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>605</v>
+        <v>634</v>
       </c>
     </row>
     <row r="6">
@@ -406,7 +406,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>413</v>
+        <v>434</v>
       </c>
     </row>
     <row r="7">
@@ -414,7 +414,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>442</v>
+        <v>458</v>
       </c>
     </row>
     <row r="8">
@@ -422,7 +422,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>474</v>
+        <v>495</v>
       </c>
     </row>
     <row r="9">
@@ -431,6 +431,38 @@
       </c>
       <c r="B9">
         <v>513</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
semana 16 de 2025
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -462,7 +462,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>369</v>
+        <v>377</v>
       </c>
     </row>
     <row r="14">
@@ -470,7 +470,39 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>432</v>
+        <v>450</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
semana 17 de 2025
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -502,7 +502,15 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>3</v>
+        <v>547</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
semana 18 de 2025
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -502,7 +502,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>547</v>
+        <v>607</v>
       </c>
     </row>
     <row r="19">
@@ -510,7 +510,15 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>5</v>
+        <v>388</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
semana 19 de 2025
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -510,7 +510,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>388</v>
+        <v>390</v>
       </c>
     </row>
     <row r="20">
@@ -518,7 +518,15 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>2</v>
+        <v>537</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
envio semana 20 de 2025
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -526,7 +526,15 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>3</v>
+        <v>305</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
semana 21 de 2025
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -534,7 +534,15 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>6</v>
+        <v>367</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
semana 24 de 2025
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -542,7 +542,31 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>290</v>
+        <v>346</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
semana 26 de 2025
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -566,7 +566,23 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>51</v>
+        <v>352</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
semana 28 de 2025
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -574,7 +574,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>225</v>
+        <v>272</v>
       </c>
     </row>
     <row r="28">
@@ -590,7 +590,15 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>47</v>
+        <v>304</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
semana 29 de 2025
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -598,7 +598,15 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>1</v>
+        <v>342</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
semana 32 de 2025
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -454,7 +454,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>556</v>
+        <v>470</v>
       </c>
     </row>
     <row r="13">
@@ -502,7 +502,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>607</v>
+        <v>457</v>
       </c>
     </row>
     <row r="19">
@@ -518,7 +518,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>537</v>
+        <v>403</v>
       </c>
     </row>
     <row r="21">
@@ -606,7 +606,31 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>372</v>
+        <v>382</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
semana 34 de 2025
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -630,7 +630,23 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>163</v>
+        <v>253</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
semana 36 de 2025
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -478,7 +478,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="16">
@@ -542,7 +542,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="24">
@@ -550,7 +550,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>357</v>
+        <v>359</v>
       </c>
     </row>
     <row r="25">
@@ -558,7 +558,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="26">
@@ -566,7 +566,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="27">
@@ -646,7 +646,15 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>1</v>
+        <v>412</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>439</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
semana 37 de 2025
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -486,7 +486,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>354</v>
+        <v>425</v>
       </c>
     </row>
     <row r="17">
@@ -654,7 +654,23 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>439</v>
+        <v>449</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
semana 38 de 2025
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B39"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -662,7 +662,7 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>503</v>
+        <v>518</v>
       </c>
     </row>
     <row r="39">
@@ -670,7 +670,15 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>1</v>
+        <v>463</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
semana 40 de 2025
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B40"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -670,7 +670,7 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>463</v>
+        <v>464</v>
       </c>
     </row>
     <row r="40">
@@ -678,7 +678,23 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <v>14</v>
+        <v>522</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
semana 41 de 2025
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -374,7 +374,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="3">
@@ -382,7 +382,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>722</v>
+        <v>719</v>
       </c>
     </row>
     <row r="4">
@@ -398,7 +398,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>634</v>
+        <v>635</v>
       </c>
     </row>
     <row r="6">
@@ -430,7 +430,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="10">
@@ -438,7 +438,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>499</v>
+        <v>496</v>
       </c>
     </row>
     <row r="11">
@@ -446,7 +446,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="12">
@@ -478,7 +478,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="16">
@@ -486,7 +486,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="17">
@@ -502,7 +502,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="19">
@@ -510,7 +510,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="20">
@@ -686,7 +686,7 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>424</v>
+        <v>480</v>
       </c>
     </row>
     <row r="42">
@@ -694,7 +694,15 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>23</v>
+        <v>272</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
semana 42 de 2025
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B43"/>
+  <dimension ref="A1:B44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -694,7 +694,7 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>272</v>
+        <v>348</v>
       </c>
     </row>
     <row r="43">
@@ -702,7 +702,15 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>3</v>
+        <v>317</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
semana epidemiologica 43 de 2025
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B44"/>
+  <dimension ref="A1:B45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -518,7 +518,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>403</v>
+        <v>400</v>
       </c>
     </row>
     <row r="21">
@@ -526,7 +526,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="22">
@@ -558,7 +558,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="26">
@@ -566,7 +566,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="27">
@@ -574,7 +574,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="28">
@@ -582,7 +582,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="29">
@@ -598,7 +598,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="31">
@@ -606,7 +606,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="32">
@@ -622,7 +622,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="34">
@@ -654,7 +654,7 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="38">
@@ -710,7 +710,15 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>56</v>
+        <v>441</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
semana 45 de 2025
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B45"/>
+  <dimension ref="A1:B47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -390,7 +390,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>432</v>
+        <v>436</v>
       </c>
     </row>
     <row r="5">
@@ -398,7 +398,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>635</v>
+        <v>637</v>
       </c>
     </row>
     <row r="6">
@@ -430,7 +430,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
     <row r="10">
@@ -454,7 +454,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>470</v>
+        <v>471</v>
       </c>
     </row>
     <row r="13">
@@ -470,7 +470,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>450</v>
+        <v>451</v>
       </c>
     </row>
     <row r="15">
@@ -502,7 +502,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>455</v>
+        <v>456</v>
       </c>
     </row>
     <row r="19">
@@ -526,7 +526,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="22">
@@ -566,7 +566,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="27">
@@ -574,7 +574,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="28">
@@ -590,7 +590,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="30">
@@ -598,7 +598,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="31">
@@ -646,7 +646,7 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="37">
@@ -654,7 +654,7 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>447</v>
+        <v>449</v>
       </c>
     </row>
     <row r="38">
@@ -686,7 +686,7 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>480</v>
+        <v>481</v>
       </c>
     </row>
     <row r="42">
@@ -718,7 +718,23 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>1</v>
+        <v>468</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
semana 46 de 2025
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
@@ -374,7 +374,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>277</v>
+        <v>311</v>
       </c>
     </row>
     <row r="3">
@@ -382,7 +382,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>719</v>
+        <v>755</v>
       </c>
     </row>
     <row r="4">
@@ -438,7 +438,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>496</v>
+        <v>497</v>
       </c>
     </row>
     <row r="11">
@@ -446,7 +446,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>581</v>
+        <v>574</v>
       </c>
     </row>
     <row r="12">
@@ -454,7 +454,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>471</v>
+        <v>473</v>
       </c>
     </row>
     <row r="13">
@@ -478,7 +478,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="16">
@@ -486,7 +486,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="17">
@@ -502,7 +502,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="19">
@@ -726,7 +726,7 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>387</v>
+        <v>417</v>
       </c>
     </row>
     <row r="47">
@@ -734,7 +734,7 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>66</v>
+        <v>438</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
semana 49 de 2025
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
@@ -398,7 +398,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="6">
@@ -406,7 +406,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>466</v>
+        <v>468</v>
       </c>
     </row>
     <row r="7">
@@ -486,7 +486,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>448</v>
+        <v>437</v>
       </c>
     </row>
     <row r="17">
@@ -494,7 +494,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="18">
@@ -502,7 +502,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="19">
@@ -510,7 +510,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="20">
@@ -518,7 +518,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="21">
@@ -526,7 +526,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>345</v>
+        <v>350</v>
       </c>
     </row>
     <row r="22">
@@ -534,7 +534,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>397</v>
+        <v>398</v>
       </c>
     </row>
     <row r="23">
@@ -542,7 +542,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="24">
@@ -550,7 +550,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="25">
@@ -558,7 +558,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>287</v>
+        <v>303</v>
       </c>
     </row>
     <row r="26">
@@ -566,7 +566,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="27">
@@ -582,7 +582,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="29">
@@ -590,7 +590,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="30">
@@ -598,7 +598,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>356</v>
+        <v>358</v>
       </c>
     </row>
     <row r="31">
@@ -670,7 +670,7 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>513</v>
+        <v>514</v>
       </c>
     </row>
     <row r="40">
@@ -758,7 +758,7 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>40</v>
+        <v>427</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
semana 50 de 2025
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B50"/>
+  <dimension ref="A1:B51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -614,7 +614,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>331</v>
+        <v>335</v>
       </c>
     </row>
     <row r="33">
@@ -622,7 +622,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="34">
@@ -630,7 +630,7 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="35">
@@ -638,7 +638,7 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>420</v>
+        <v>423</v>
       </c>
     </row>
     <row r="36">
@@ -654,7 +654,7 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>484</v>
+        <v>489</v>
       </c>
     </row>
     <row r="38">
@@ -718,7 +718,7 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>483</v>
+        <v>429</v>
       </c>
     </row>
     <row r="46">
@@ -726,7 +726,7 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="47">
@@ -758,7 +758,15 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>427</v>
+        <v>445</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>431</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
semana 52 de 2025
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B51"/>
+  <dimension ref="A1:B54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -374,7 +374,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>316</v>
+        <v>306</v>
       </c>
     </row>
     <row r="3">
@@ -382,7 +382,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>755</v>
+        <v>469</v>
       </c>
     </row>
     <row r="4">
@@ -390,7 +390,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>471</v>
+        <v>479</v>
       </c>
     </row>
     <row r="5">
@@ -398,7 +398,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>683</v>
+        <v>673</v>
       </c>
     </row>
     <row r="6">
@@ -406,7 +406,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>468</v>
+        <v>481</v>
       </c>
     </row>
     <row r="7">
@@ -414,7 +414,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>506</v>
+        <v>535</v>
       </c>
     </row>
     <row r="8">
@@ -422,7 +422,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>527</v>
+        <v>538</v>
       </c>
     </row>
     <row r="9">
@@ -430,7 +430,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>569</v>
+        <v>588</v>
       </c>
     </row>
     <row r="10">
@@ -438,7 +438,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>524</v>
+        <v>533</v>
       </c>
     </row>
     <row r="11">
@@ -446,7 +446,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>573</v>
+        <v>601</v>
       </c>
     </row>
     <row r="12">
@@ -454,7 +454,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>507</v>
+        <v>524</v>
       </c>
     </row>
     <row r="13">
@@ -462,7 +462,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>416</v>
+        <v>433</v>
       </c>
     </row>
     <row r="14">
@@ -470,7 +470,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>478</v>
+        <v>490</v>
       </c>
     </row>
     <row r="15">
@@ -478,7 +478,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>500</v>
+        <v>513</v>
       </c>
     </row>
     <row r="16">
@@ -486,7 +486,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>437</v>
+        <v>458</v>
       </c>
     </row>
     <row r="17">
@@ -494,7 +494,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>274</v>
+        <v>291</v>
       </c>
     </row>
     <row r="18">
@@ -502,7 +502,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>482</v>
+        <v>492</v>
       </c>
     </row>
     <row r="19">
@@ -510,7 +510,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>410</v>
+        <v>423</v>
       </c>
     </row>
     <row r="20">
@@ -518,7 +518,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>426</v>
+        <v>441</v>
       </c>
     </row>
     <row r="21">
@@ -526,7 +526,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>350</v>
+        <v>368</v>
       </c>
     </row>
     <row r="22">
@@ -534,7 +534,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>398</v>
+        <v>416</v>
       </c>
     </row>
     <row r="23">
@@ -542,7 +542,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>389</v>
+        <v>407</v>
       </c>
     </row>
     <row r="24">
@@ -550,7 +550,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>383</v>
+        <v>395</v>
       </c>
     </row>
     <row r="25">
@@ -558,7 +558,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>303</v>
+        <v>315</v>
       </c>
     </row>
     <row r="26">
@@ -566,7 +566,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>377</v>
+        <v>385</v>
       </c>
     </row>
     <row r="27">
@@ -574,7 +574,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>280</v>
+        <v>292</v>
       </c>
     </row>
     <row r="28">
@@ -582,7 +582,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>255</v>
+        <v>269</v>
       </c>
     </row>
     <row r="29">
@@ -590,7 +590,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>350</v>
+        <v>368</v>
       </c>
     </row>
     <row r="30">
@@ -598,7 +598,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>358</v>
+        <v>377</v>
       </c>
     </row>
     <row r="31">
@@ -606,7 +606,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>448</v>
+        <v>470</v>
       </c>
     </row>
     <row r="32">
@@ -614,7 +614,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>335</v>
+        <v>346</v>
       </c>
     </row>
     <row r="33">
@@ -622,7 +622,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>275</v>
+        <v>290</v>
       </c>
     </row>
     <row r="34">
@@ -630,7 +630,7 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>309</v>
+        <v>323</v>
       </c>
     </row>
     <row r="35">
@@ -638,7 +638,7 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>423</v>
+        <v>434</v>
       </c>
     </row>
     <row r="36">
@@ -646,7 +646,7 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>449</v>
+        <v>466</v>
       </c>
     </row>
     <row r="37">
@@ -654,7 +654,7 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>489</v>
+        <v>510</v>
       </c>
     </row>
     <row r="38">
@@ -662,7 +662,7 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>557</v>
+        <v>580</v>
       </c>
     </row>
     <row r="39">
@@ -670,7 +670,7 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>514</v>
+        <v>526</v>
       </c>
     </row>
     <row r="40">
@@ -678,7 +678,7 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <v>545</v>
+        <v>557</v>
       </c>
     </row>
     <row r="41">
@@ -686,7 +686,7 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>498</v>
+        <v>517</v>
       </c>
     </row>
     <row r="42">
@@ -694,7 +694,7 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>379</v>
+        <v>392</v>
       </c>
     </row>
     <row r="43">
@@ -702,7 +702,7 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>331</v>
+        <v>347</v>
       </c>
     </row>
     <row r="44">
@@ -710,7 +710,7 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>456</v>
+        <v>478</v>
       </c>
     </row>
     <row r="45">
@@ -718,7 +718,7 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>429</v>
+        <v>447</v>
       </c>
     </row>
     <row r="46">
@@ -726,7 +726,7 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>439</v>
+        <v>451</v>
       </c>
     </row>
     <row r="47">
@@ -734,7 +734,7 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>457</v>
+        <v>484</v>
       </c>
     </row>
     <row r="48">
@@ -742,7 +742,7 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>381</v>
+        <v>400</v>
       </c>
     </row>
     <row r="49">
@@ -750,7 +750,7 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>457</v>
+        <v>468</v>
       </c>
     </row>
     <row r="50">
@@ -758,7 +758,7 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>445</v>
+        <v>458</v>
       </c>
     </row>
     <row r="51">
@@ -766,7 +766,31 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>431</v>
+        <v>446</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
semana 5 de 2026
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -406,7 +406,15 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>51</v>
+        <v>499</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
semana 6 de 2026
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/eda2018.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -414,7 +414,15 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>451</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>